<commit_message>
fix(import): update date-time format & edit data
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_stok.xlsx
+++ b/PWL_POS/public/template_stok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\= KULIAH\SEMESTER 4\3. PRAK JOBSHEET\PWL25\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F467FB-96CA-4D12-9D1B-8D30BDE72016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4211757-F531-4B9D-BD7F-658383F8001A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{71D03154-FC80-4616-B54F-B5EF813E3D2D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>barang_id</t>
   </si>
@@ -46,16 +46,13 @@
   <si>
     <t>jumlah</t>
   </si>
-  <si>
-    <t>stok_tanggal</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -97,8 +94,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +433,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,9 +452,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -468,9 +463,6 @@
       </c>
       <c r="C2">
         <v>33</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>